<commit_message>
Risolto bug HMR e aggiunti altri log per il debug
</commit_message>
<xml_diff>
--- a/progetti-per-test/Progetto-Complesso-V1/confronto-pratiche.xlsx
+++ b/progetti-per-test/Progetto-Complesso-V1/confronto-pratiche.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIN10\Desktop\Tirocinio-Aggiornato\progetti-per-test\Progetto-Complesso-V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIN10\Desktop\Tirocinio-aggiornato\progetti-per-test\Progetto-Complesso-V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -978,7 +978,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
@@ -1081,14 +1083,14 @@
         <v>36</v>
       </c>
       <c r="E6" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>15.909090909090908</v>
+        <v>6.8181818181818175</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1234,14 +1236,14 @@
         <v>34</v>
       </c>
       <c r="E13" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>21.739130434782609</v>
+        <v>6.5217391304347823</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1365,7 +1367,7 @@
       </c>
       <c r="B20" s="1">
         <f>SUM(E4:E9)</f>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1">
         <f>SUM(F4:F9)</f>
@@ -1373,7 +1375,7 @@
       </c>
       <c r="D20" s="1">
         <f>SUM(B20,C20)</f>
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E20" s="1">
         <v>3</v>
@@ -1391,7 +1393,7 @@
       </c>
       <c r="B21" s="1">
         <f>SUM(E11:E16)</f>
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1">
         <f>SUM(F11:F16)</f>
@@ -1399,7 +1401,7 @@
       </c>
       <c r="D21" s="1">
         <f>SUM(B21,C21)</f>
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Testato progetto HTML con locatori generati con il tool per robula+
</commit_message>
<xml_diff>
--- a/progetti-per-test/Progetto-Complesso-V1/confronto-pratiche.xlsx
+++ b/progetti-per-test/Progetto-Complesso-V1/confronto-pratiche.xlsx
@@ -979,7 +979,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1233,7 +1233,7 @@
         <v>46</v>
       </c>
       <c r="D13" s="1">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1">
         <v>3</v>

</xml_diff>